<commit_message>
generated stats for great league
</commit_message>
<xml_diff>
--- a/data/raw/moves.xlsx
+++ b/data/raw/moves.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nrhod\Documents\Coding\Python\pogoevo\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b87db9f3afdc293/Documents/Coding/Python/pogoevo/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9D1C95-F79B-4A41-A632-D5FC63A82658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{5A9D1C95-F79B-4A41-A632-D5FC63A82658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BE946D6-A891-4473-BC43-D68E5B3E2B25}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{C7818452-25B9-4EE3-A75F-5102B69A1898}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C7818452-25B9-4EE3-A75F-5102B69A1898}"/>
   </bookViews>
   <sheets>
     <sheet name="charge" sheetId="2" r:id="rId1"/>
     <sheet name="fast" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">charge!$A$1:$H$164</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">charge!$A$1:$H$165</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">fast!$A$1:$H$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="256">
   <si>
     <t>MOVE</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Lick</t>
   </si>
   <si>
-    <t>Lock On</t>
-  </si>
-  <si>
     <t>Low Kick</t>
   </si>
   <si>
@@ -493,9 +490,6 @@
     <t>Frustration</t>
   </si>
   <si>
-    <t>Futuresight</t>
-  </si>
-  <si>
     <t>Giga Drain</t>
   </si>
   <si>
@@ -637,9 +631,6 @@
     <t>Power Gem</t>
   </si>
   <si>
-    <t>Power Up Punch</t>
-  </si>
-  <si>
     <t>Power Whip</t>
   </si>
   <si>
@@ -742,9 +733,6 @@
     <t>Submission</t>
   </si>
   <si>
-    <t>Super Power</t>
-  </si>
-  <si>
     <t>Surf</t>
   </si>
   <si>
@@ -766,9 +754,6 @@
     <t>Twister</t>
   </si>
   <si>
-    <t>Vice Grip</t>
-  </si>
-  <si>
     <t>Water Pulse</t>
   </si>
   <si>
@@ -796,13 +781,31 @@
     <t>Wrap Pink</t>
   </si>
   <si>
-    <t>X Scissor</t>
-  </si>
-  <si>
     <t>Zap Cannon</t>
   </si>
   <si>
     <t>DMG/ENG</t>
+  </si>
+  <si>
+    <t>X-Scissor</t>
+  </si>
+  <si>
+    <t>Power-Up Punch</t>
+  </si>
+  <si>
+    <t>Future Sight</t>
+  </si>
+  <si>
+    <t>Vise Grip</t>
+  </si>
+  <si>
+    <t>Superpower</t>
+  </si>
+  <si>
+    <t>Lock-On</t>
+  </si>
+  <si>
+    <t>Weather Ball</t>
   </si>
 </sst>
 </file>
@@ -1155,25 +1158,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197F016C-B031-4DCB-ACD9-D4BABA4AD53F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H162"/>
+  <dimension ref="A1:H163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.06640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1196,15 +1199,15 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -1225,12 +1228,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>55</v>
@@ -1251,12 +1254,12 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4">
         <v>60</v>
@@ -1277,12 +1280,12 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5">
         <v>45</v>
@@ -1303,12 +1306,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6">
         <v>45</v>
@@ -1329,12 +1332,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7">
         <v>50</v>
@@ -1355,12 +1358,12 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -1381,12 +1384,12 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9">
         <v>80</v>
@@ -1407,12 +1410,12 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10">
         <v>90</v>
@@ -1433,12 +1436,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11">
         <v>110</v>
@@ -1459,12 +1462,12 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12">
         <v>55</v>
@@ -1485,12 +1488,12 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13">
         <v>130</v>
@@ -1511,12 +1514,12 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14">
         <v>60</v>
@@ -1537,12 +1540,12 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15">
         <v>40</v>
@@ -1563,12 +1566,12 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16">
         <v>90</v>
@@ -1589,12 +1592,12 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17">
         <v>40</v>
@@ -1615,12 +1618,12 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18">
         <v>60</v>
@@ -1641,12 +1644,12 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19">
         <v>25</v>
@@ -1667,12 +1670,12 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20">
         <v>90</v>
@@ -1693,12 +1696,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21">
         <v>80</v>
@@ -1719,12 +1722,12 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22">
         <v>100</v>
@@ -1745,12 +1748,12 @@
         <v>2.2200000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23">
         <v>75</v>
@@ -1771,12 +1774,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24">
         <v>50</v>
@@ -1797,12 +1800,12 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25">
         <v>40</v>
@@ -1823,12 +1826,12 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26">
         <v>70</v>
@@ -1849,12 +1852,12 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1875,12 +1878,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28">
         <v>80</v>
@@ -1901,12 +1904,12 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C29">
         <v>110</v>
@@ -1927,12 +1930,12 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30">
         <v>100</v>
@@ -1953,12 +1956,12 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31">
         <v>70</v>
@@ -1979,12 +1982,12 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32">
         <v>65</v>
@@ -2005,12 +2008,12 @@
         <v>1.44</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C33">
         <v>75</v>
@@ -2031,12 +2034,12 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34">
         <v>150</v>
@@ -2057,12 +2060,12 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35">
         <v>50</v>
@@ -2083,12 +2086,12 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36">
         <v>90</v>
@@ -2109,12 +2112,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2135,12 +2138,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38">
         <v>60</v>
@@ -2161,12 +2164,12 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39">
         <v>60</v>
@@ -2187,12 +2190,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C40">
         <v>80</v>
@@ -2213,12 +2216,12 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C41">
         <v>90</v>
@@ -2239,12 +2242,12 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C42">
         <v>90</v>
@@ -2265,12 +2268,12 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C43">
         <v>120</v>
@@ -2291,12 +2294,12 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C44">
         <v>90</v>
@@ -2317,12 +2320,12 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45">
         <v>20</v>
@@ -2343,12 +2346,12 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46">
         <v>140</v>
@@ -2369,12 +2372,12 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47">
         <v>55</v>
@@ -2395,12 +2398,12 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2421,12 +2424,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C49">
         <v>70</v>
@@ -2447,12 +2450,12 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C50">
         <v>70</v>
@@ -2473,12 +2476,12 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C51">
         <v>60</v>
@@ -2499,12 +2502,12 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C52">
         <v>90</v>
@@ -2525,12 +2528,12 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53">
         <v>110</v>
@@ -2551,12 +2554,12 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54">
         <v>90</v>
@@ -2577,12 +2580,12 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55">
         <v>150</v>
@@ -2603,12 +2606,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C56">
         <v>70</v>
@@ -2629,12 +2632,12 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C57">
         <v>100</v>
@@ -2655,12 +2658,12 @@
         <v>2.2200000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58">
         <v>10</v>
@@ -2681,12 +2684,12 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>251</v>
       </c>
       <c r="B59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C59">
         <v>120</v>
@@ -2707,12 +2710,12 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C60">
         <v>50</v>
@@ -2733,12 +2736,12 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C61">
         <v>150</v>
@@ -2759,12 +2762,12 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C62">
         <v>90</v>
@@ -2785,12 +2788,12 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63">
         <v>130</v>
@@ -2811,12 +2814,12 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C64">
         <v>80</v>
@@ -2837,12 +2840,12 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C65">
         <v>40</v>
@@ -2863,12 +2866,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C66">
         <v>95</v>
@@ -2889,12 +2892,12 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C67">
         <v>70</v>
@@ -2915,12 +2918,12 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68">
         <v>40</v>
@@ -2941,12 +2944,12 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2967,12 +2970,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C70">
         <v>110</v>
@@ -2993,12 +2996,12 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C71">
         <v>80</v>
@@ -3019,12 +3022,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C72">
         <v>130</v>
@@ -3045,12 +3048,12 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C73">
         <v>90</v>
@@ -3071,12 +3074,12 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B74" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C74">
         <v>150</v>
@@ -3097,12 +3100,12 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C75">
         <v>80</v>
@@ -3123,12 +3126,12 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C76">
         <v>90</v>
@@ -3149,12 +3152,12 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C77">
         <v>55</v>
@@ -3175,12 +3178,12 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C78">
         <v>60</v>
@@ -3201,12 +3204,12 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C79">
         <v>70</v>
@@ -3227,12 +3230,12 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B80" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C80">
         <v>90</v>
@@ -3253,12 +3256,12 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C81">
         <v>70</v>
@@ -3279,12 +3282,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C82">
         <v>45</v>
@@ -3305,12 +3308,12 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B83" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -3331,12 +3334,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B84" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C84">
         <v>40</v>
@@ -3357,12 +3360,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B85" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -3383,12 +3386,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B86" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C86">
         <v>70</v>
@@ -3409,12 +3412,12 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C87">
         <v>25</v>
@@ -3435,12 +3438,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B88" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C88">
         <v>100</v>
@@ -3461,12 +3464,12 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B89" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C89">
         <v>100</v>
@@ -3487,12 +3490,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B90" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C90">
         <v>60</v>
@@ -3513,12 +3516,12 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B91" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C91">
         <v>35</v>
@@ -3539,12 +3542,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B92" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C92">
         <v>110</v>
@@ -3565,12 +3568,12 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B93" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C93">
         <v>55</v>
@@ -3591,12 +3594,12 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C94">
         <v>35</v>
@@ -3617,12 +3620,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B95" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C95">
         <v>60</v>
@@ -3643,12 +3646,12 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B96" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C96">
         <v>50</v>
@@ -3669,12 +3672,12 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B97" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C97">
         <v>50</v>
@@ -3695,12 +3698,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B98" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C98">
         <v>45</v>
@@ -3721,12 +3724,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B99" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C99">
         <v>130</v>
@@ -3747,12 +3750,12 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C100">
         <v>110</v>
@@ -3773,12 +3776,12 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C101">
         <v>130</v>
@@ -3799,12 +3802,12 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B102" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C102">
         <v>25</v>
@@ -3825,12 +3828,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B103" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C103">
         <v>110</v>
@@ -3851,12 +3854,12 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B104" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C104">
         <v>90</v>
@@ -3877,12 +3880,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B105" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C105">
         <v>40</v>
@@ -3903,12 +3906,12 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B106" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C106">
         <v>80</v>
@@ -3929,12 +3932,12 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>199</v>
+        <v>250</v>
       </c>
       <c r="B107" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C107">
         <v>20</v>
@@ -3955,12 +3958,12 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B108" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C108">
         <v>90</v>
@@ -3981,12 +3984,12 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C109">
         <v>130</v>
@@ -4007,12 +4010,12 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B110" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C110">
         <v>70</v>
@@ -4033,12 +4036,12 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B111" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C111">
         <v>90</v>
@@ -4059,12 +4062,12 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B112" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C112">
         <v>70</v>
@@ -4085,12 +4088,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B113" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C113">
         <v>70</v>
@@ -4111,12 +4114,12 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B114" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C114">
         <v>90</v>
@@ -4137,12 +4140,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B115" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -4163,12 +4166,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B116" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C116">
         <v>50</v>
@@ -4189,12 +4192,12 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B117" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C117">
         <v>130</v>
@@ -4215,12 +4218,12 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B118" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C118">
         <v>50</v>
@@ -4241,12 +4244,12 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B119" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C119">
         <v>80</v>
@@ -4267,12 +4270,12 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B120" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C120">
         <v>70</v>
@@ -4293,12 +4296,12 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B121" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C121">
         <v>110</v>
@@ -4319,12 +4322,12 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B122" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C122">
         <v>60</v>
@@ -4345,12 +4348,12 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B123" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C123">
         <v>25</v>
@@ -4371,12 +4374,12 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B124" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C124">
         <v>80</v>
@@ -4397,12 +4400,12 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B125" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C125">
         <v>50</v>
@@ -4423,12 +4426,12 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B126" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C126">
         <v>55</v>
@@ -4449,12 +4452,12 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B127" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C127">
         <v>100</v>
@@ -4475,12 +4478,12 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B128" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -4501,12 +4504,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B129" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C129">
         <v>40</v>
@@ -4527,12 +4530,12 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B130" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C130">
         <v>50</v>
@@ -4553,12 +4556,12 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B131" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C131">
         <v>75</v>
@@ -4579,12 +4582,12 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B132" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C132">
         <v>45</v>
@@ -4605,12 +4608,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B133" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C133">
         <v>130</v>
@@ -4631,12 +4634,12 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B134" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C134">
         <v>80</v>
@@ -4657,12 +4660,12 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B135" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C135">
         <v>50</v>
@@ -4683,12 +4686,12 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B136" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C136">
         <v>80</v>
@@ -4709,12 +4712,12 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B137" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C137">
         <v>110</v>
@@ -4735,12 +4738,12 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B138" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C138">
         <v>150</v>
@@ -4761,12 +4764,12 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B139" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C139">
         <v>55</v>
@@ -4787,12 +4790,12 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B140" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C140">
         <v>100</v>
@@ -4813,12 +4816,12 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B141" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C141">
         <v>35</v>
@@ -4839,12 +4842,12 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B142" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C142">
         <v>60</v>
@@ -4865,12 +4868,12 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="B143" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C143">
         <v>85</v>
@@ -4891,12 +4894,12 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B144" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C144">
         <v>65</v>
@@ -4917,12 +4920,12 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B145" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C145">
         <v>60</v>
@@ -4943,12 +4946,12 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B146" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C146">
         <v>80</v>
@@ -4969,12 +4972,12 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B147" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C147">
         <v>100</v>
@@ -4995,12 +4998,12 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B148" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C148">
         <v>55</v>
@@ -5021,12 +5024,12 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B149" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C149">
         <v>90</v>
@@ -5047,12 +5050,12 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B150" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C150">
         <v>45</v>
@@ -5073,12 +5076,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="B151" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C151">
         <v>40</v>
@@ -5099,12 +5102,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B152" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C152">
         <v>70</v>
@@ -5125,12 +5128,12 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="B153" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C153">
         <v>60</v>
@@ -5151,12 +5154,12 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B154" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C154">
         <v>60</v>
@@ -5177,12 +5180,12 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B155" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C155">
         <v>60</v>
@@ -5203,12 +5206,12 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B156" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C156">
         <v>60</v>
@@ -5229,41 +5232,41 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B157" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C157">
+        <v>60</v>
+      </c>
+      <c r="D157">
+        <v>35</v>
+      </c>
+      <c r="E157">
+        <v>6</v>
+      </c>
+      <c r="F157">
+        <v>10</v>
+      </c>
+      <c r="G157">
+        <v>5.83</v>
+      </c>
+      <c r="H157">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>243</v>
+      </c>
+      <c r="B158" t="s">
+        <v>78</v>
+      </c>
+      <c r="C158">
         <v>100</v>
-      </c>
-      <c r="D157">
-        <v>45</v>
-      </c>
-      <c r="E157">
-        <v>6</v>
-      </c>
-      <c r="F157">
-        <v>16.670000000000002</v>
-      </c>
-      <c r="G157">
-        <v>7.5</v>
-      </c>
-      <c r="H157">
-        <v>2.2200000000000002</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A158" t="s">
-        <v>249</v>
-      </c>
-      <c r="B158" t="s">
-        <v>88</v>
-      </c>
-      <c r="C158">
-        <v>60</v>
       </c>
       <c r="D158">
         <v>45</v>
@@ -5272,24 +5275,24 @@
         <v>6</v>
       </c>
       <c r="F158">
-        <v>10</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="G158">
         <v>7.5</v>
       </c>
       <c r="H158">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.45">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B159" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C159">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="D159">
         <v>45</v>
@@ -5298,21 +5301,21 @@
         <v>6</v>
       </c>
       <c r="F159">
-        <v>4.17</v>
+        <v>10</v>
       </c>
       <c r="G159">
         <v>7.5</v>
       </c>
       <c r="H159">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.45">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B160" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C160">
         <v>25</v>
@@ -5333,55 +5336,81 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B161" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C161">
+        <v>25</v>
+      </c>
+      <c r="D161">
         <v>45</v>
       </c>
-      <c r="D161">
+      <c r="E161">
+        <v>6</v>
+      </c>
+      <c r="F161">
+        <v>4.17</v>
+      </c>
+      <c r="G161">
+        <v>7.5</v>
+      </c>
+      <c r="H161">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>249</v>
+      </c>
+      <c r="B162" t="s">
+        <v>75</v>
+      </c>
+      <c r="C162">
+        <v>45</v>
+      </c>
+      <c r="D162">
         <v>35</v>
       </c>
-      <c r="E161">
-        <v>6</v>
-      </c>
-      <c r="F161">
+      <c r="E162">
+        <v>6</v>
+      </c>
+      <c r="F162">
         <v>7.5</v>
       </c>
-      <c r="G161">
+      <c r="G162">
         <v>5.83</v>
       </c>
-      <c r="H161">
+      <c r="H162">
         <v>1.29</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A162" t="s">
-        <v>253</v>
-      </c>
-      <c r="B162" t="s">
-        <v>79</v>
-      </c>
-      <c r="C162">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>247</v>
+      </c>
+      <c r="B163" t="s">
+        <v>78</v>
+      </c>
+      <c r="C163">
         <v>150</v>
       </c>
-      <c r="D162">
+      <c r="D163">
         <v>80</v>
       </c>
-      <c r="E162">
-        <v>6</v>
-      </c>
-      <c r="F162">
+      <c r="E163">
+        <v>6</v>
+      </c>
+      <c r="F163">
         <v>25</v>
       </c>
-      <c r="G162">
+      <c r="G163">
         <v>13.33</v>
       </c>
-      <c r="H162">
+      <c r="H163">
         <v>1.88</v>
       </c>
     </row>
@@ -5398,21 +5427,21 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5438,12 +5467,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -5464,12 +5493,12 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>9</v>
@@ -5490,12 +5519,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -5516,12 +5545,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -5542,12 +5571,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -5568,12 +5597,12 @@
         <v>9.7799999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -5594,12 +5623,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -5620,12 +5649,12 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -5646,12 +5675,12 @@
         <v>7.22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -5672,12 +5701,12 @@
         <v>6.11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11">
         <v>16</v>
@@ -5698,12 +5727,12 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12">
         <v>16</v>
@@ -5724,12 +5753,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13">
         <v>8</v>
@@ -5750,12 +5779,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -5776,12 +5805,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -5802,12 +5831,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16">
         <v>9</v>
@@ -5828,12 +5857,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -5854,12 +5883,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18">
         <v>8</v>
@@ -5880,12 +5909,12 @@
         <v>8.89</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19">
         <v>6</v>
@@ -5906,12 +5935,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -5932,12 +5961,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21">
         <v>9</v>
@@ -5958,12 +5987,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22">
         <v>7</v>
@@ -5984,12 +6013,12 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -6010,12 +6039,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24">
         <v>6</v>
@@ -6036,12 +6065,12 @@
         <v>7.33</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25">
         <v>9</v>
@@ -6062,12 +6091,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26">
         <v>8</v>
@@ -6088,12 +6117,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27">
         <v>9</v>
@@ -6114,12 +6143,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28">
         <v>6</v>
@@ -6140,12 +6169,12 @@
         <v>7.33</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29">
         <v>9</v>
@@ -6166,12 +6195,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -6192,12 +6221,12 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -6218,12 +6247,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>254</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -6244,12 +6273,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -6270,12 +6299,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C34">
         <v>5</v>
@@ -6296,12 +6325,12 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -6322,12 +6351,12 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36">
         <v>11</v>
@@ -6348,12 +6377,12 @@
         <v>9.7799999999999994</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37">
         <v>6</v>
@@ -6374,12 +6403,12 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38">
         <v>6</v>
@@ -6400,12 +6429,12 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -6426,12 +6455,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40">
         <v>5</v>
@@ -6452,12 +6481,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -6478,12 +6507,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42">
         <v>3</v>
@@ -6504,12 +6533,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C43">
         <v>3</v>
@@ -6530,12 +6559,12 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44">
         <v>5</v>
@@ -6556,12 +6585,12 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C45">
         <v>11</v>
@@ -6582,12 +6611,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46">
         <v>9</v>
@@ -6608,12 +6637,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C47">
         <v>8</v>
@@ -6634,12 +6663,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C48">
         <v>4</v>
@@ -6660,12 +6689,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49">
         <v>6</v>
@@ -6686,12 +6715,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C50">
         <v>12</v>
@@ -6712,12 +6741,12 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C51">
         <v>5</v>
@@ -6738,12 +6767,12 @@
         <v>7.22</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C52">
         <v>4</v>
@@ -6764,12 +6793,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -6790,12 +6819,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C54">
         <v>7</v>
@@ -6816,12 +6845,12 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55">
         <v>9</v>
@@ -6842,12 +6871,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C56">
         <v>5</v>
@@ -6868,12 +6897,12 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C57">
         <v>3</v>
@@ -6894,12 +6923,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58">
         <v>5</v>
@@ -6920,12 +6949,12 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C59">
         <v>8</v>
@@ -6946,12 +6975,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C60">
         <v>3</v>
@@ -6972,12 +7001,12 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -6998,12 +7027,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C62">
         <v>5</v>
@@ -7024,12 +7053,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C63">
         <v>12</v>
@@ -7050,12 +7079,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C64">
         <v>3</v>
@@ -7076,12 +7105,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C65">
         <v>6</v>
@@ -7102,12 +7131,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C66">
         <v>12</v>
@@ -7128,12 +7157,12 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C67">
         <v>5</v>
@@ -7154,12 +7183,12 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -7180,12 +7209,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B69" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C69">
         <v>8</v>

</xml_diff>